<commit_message>
created customer annontation to set test author and category
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -87,8 +87,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -108,53 +108,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,46 +214,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,37 +251,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -267,19 +267,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,6 +405,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -303,151 +423,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,6 +458,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -485,50 +535,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,17 +558,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -566,149 +566,149 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -720,6 +720,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1060,19 +1063,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1122,7 +1125,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1187,8 +1190,8 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
added password decoder util
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -69,7 +69,7 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
+    <t>YWRtaW4xMjM=</t>
   </si>
   <si>
     <t>no</t>
@@ -87,9 +87,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -108,22 +108,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,61 +118,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,7 +141,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,15 +194,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,6 +221,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -267,13 +267,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,25 +393,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,139 +447,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,11 +461,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,6 +487,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,35 +532,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,17 +548,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,148 +563,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1133,6 +1133,7 @@
     <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="9.66666666666667" customWidth="1"/>
     <col min="4" max="4" width="10.2222222222222" customWidth="1"/>
+    <col min="5" max="5" width="16.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1216,7 +1217,7 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created driver factory and added custome annotation to logintest
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14004" windowHeight="3900" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNNERMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:E3"/>
 </workbook>
 </file>
 
@@ -75,10 +74,10 @@
     <t>no</t>
   </si>
   <si>
+    <t>Admin1</t>
+  </si>
+  <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>Admin1</t>
   </si>
 </sst>
 </file>
@@ -87,9 +86,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -108,14 +107,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -124,9 +115,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,45 +153,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,23 +183,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,30 +199,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,31 +266,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,145 +434,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,36 +457,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -502,15 +471,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,11 +499,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,153 +533,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,7 +1048,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1125,7 +1124,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1181,7 +1180,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>17</v>
@@ -1192,13 +1191,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -1212,10 +1211,10 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>

</xml_diff>